<commit_message>
finalizando los estilos - empezando con script de base
</commit_message>
<xml_diff>
--- a/Reporte Operadores s2s - Mera.xlsx
+++ b/Reporte Operadores s2s - Mera.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -45,8 +45,18 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+      <sz val="22"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -57,6 +67,12 @@
       <patternFill patternType="solid">
         <fgColor theme="3"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0044546A"/>
+        <bgColor rgb="0044546A"/>
       </patternFill>
     </fill>
   </fills>
@@ -87,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -103,6 +119,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -482,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H95"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,224 +523,54 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="B1" s="7" t="inlineStr">
+        <is>
+          <t>OPERADORES S2S - CSV MERA</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
+    <row r="3"/>
+    <row r="4"/>
+    <row r="6">
+      <c r="A6" s="8" t="inlineStr">
         <is>
           <t>PCRC</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B6" s="8" t="inlineStr">
         <is>
           <t>OPERADOR</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C6" s="8" t="inlineStr">
         <is>
           <t>Cod. Agente</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D6" s="8" t="inlineStr">
         <is>
           <t>Ll. ACD</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E6" s="8" t="inlineStr">
         <is>
           <t>LOGUEO</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F6" s="8" t="inlineStr">
         <is>
           <t>Q. Ventas</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G6" s="8" t="inlineStr">
         <is>
           <t>vma</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H6" s="8" t="inlineStr">
         <is>
           <t>Supervisor</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>S2S NO PREMIUM</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>ACOSTA AYELEN</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>605502</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
-        <is>
-          <t>14:00 - 15:00</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>VMAAYACO</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>VILLALBA, VICTORIA</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>S2S NO PREMIUM</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>ACOSTA SEBASTIAN</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>606264</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="inlineStr">
-        <is>
-          <t>14:00 - 15:30</t>
-        </is>
-      </c>
-      <c r="F3" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G3" s="2" t="inlineStr">
-        <is>
-          <t>VMASEACO</t>
-        </is>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>ROJAS, LUCAS</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>S2S NO PREMIUM</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>ALMIRON LUCIANA AYELEN</t>
-        </is>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>606470</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="inlineStr">
-        <is>
-          <t>14:30 - 20:00</t>
-        </is>
-      </c>
-      <c r="F4" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G4" s="2" t="inlineStr">
-        <is>
-          <t>VMALUALM</t>
-        </is>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>YBARRA, LUCIA ALDANA</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>S2S NO PREMIUM</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>AMUNDARREY JOAQUIN LEONEL</t>
-        </is>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>665673</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="inlineStr">
-        <is>
-          <t>14:00 - 15:30</t>
-        </is>
-      </c>
-      <c r="F5" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G5" s="2" t="inlineStr">
-        <is>
-          <t>VMAJOAMU</t>
-        </is>
-      </c>
-      <c r="H5" s="2" t="inlineStr">
-        <is>
-          <t>ROBLEDO, YESICA DANIELA</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>S2S NO PREMIUM</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="inlineStr">
-        <is>
-          <t>ANDRZEYEVSKI NICOLOSI CAMILA BELEN</t>
-        </is>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>606649</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="inlineStr">
-        <is>
-          <t>14:00 - 15:00</t>
-        </is>
-      </c>
-      <c r="F6" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G6" s="2" t="inlineStr">
-        <is>
-          <t>VMACAAND</t>
-        </is>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>DIAZ, PAULA</t>
         </is>
       </c>
     </row>
@@ -730,18 +582,18 @@
       </c>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>BARROJO FEDERICO ALEJANDRO</t>
+          <t>ACOSTA AYELEN</t>
         </is>
       </c>
       <c r="C7" s="5" t="n">
-        <v>606507</v>
+        <v>605502</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E7" s="2" t="inlineStr">
         <is>
-          <t>18:00 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F7" s="2" t="n">
@@ -749,12 +601,12 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>VMAFEBAR</t>
+          <t>VMAAYACO</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
         <is>
-          <t>MIR, TOMAS MAURICIO</t>
+          <t>VILLALBA, VICTORIA</t>
         </is>
       </c>
     </row>
@@ -766,14 +618,14 @@
       </c>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>BELCHIOR MEDINACELLI LUZ MARIA</t>
+          <t>ACOSTA SEBASTIAN</t>
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>606408</v>
+        <v>606264</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="inlineStr">
         <is>
@@ -785,7 +637,7 @@
       </c>
       <c r="G8" s="2" t="inlineStr">
         <is>
-          <t>VMALUBEL</t>
+          <t>VMASEACO</t>
         </is>
       </c>
       <c r="H8" s="2" t="inlineStr">
@@ -802,18 +654,18 @@
       </c>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>BERTUCCI AGOSTINA</t>
+          <t>ALMIRON LUCIANA AYELEN</t>
         </is>
       </c>
       <c r="C9" s="5" t="n">
-        <v>605591</v>
+        <v>606470</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F9" s="2" t="n">
@@ -821,12 +673,12 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>vmaagber</t>
+          <t>VMALUALM</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
         <is>
-          <t>ROBLEDO, YESICA DANIELA</t>
+          <t>YBARRA, LUCIA ALDANA</t>
         </is>
       </c>
     </row>
@@ -838,18 +690,18 @@
       </c>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>BURSESE MAITE PILAR</t>
+          <t>AMUNDARREY JOAQUIN LEONEL</t>
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>606443</v>
+        <v>665673</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E10" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 16:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F10" s="2" t="n">
@@ -857,12 +709,12 @@
       </c>
       <c r="G10" s="2" t="inlineStr">
         <is>
-          <t>VMAMABUR</t>
+          <t>VMAJOAMU</t>
         </is>
       </c>
       <c r="H10" s="2" t="inlineStr">
         <is>
-          <t>ROJAS, LUCAS</t>
+          <t>ROBLEDO, YESICA DANIELA</t>
         </is>
       </c>
     </row>
@@ -874,18 +726,18 @@
       </c>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>CALAHUANA SILVANA</t>
+          <t>ANDRZEYEVSKI NICOLOSI CAMILA BELEN</t>
         </is>
       </c>
       <c r="C11" s="5" t="n">
-        <v>606371</v>
+        <v>606649</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E11" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 18:30</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F11" s="2" t="n">
@@ -893,12 +745,12 @@
       </c>
       <c r="G11" s="2" t="inlineStr">
         <is>
-          <t>VMASICAL</t>
+          <t>VMACAAND</t>
         </is>
       </c>
       <c r="H11" s="2" t="inlineStr">
         <is>
-          <t>SOLER, SANTIAGO MAXIMILIANO</t>
+          <t>DIAZ, PAULA</t>
         </is>
       </c>
     </row>
@@ -910,18 +762,18 @@
       </c>
       <c r="B12" s="5" t="inlineStr">
         <is>
-          <t>CANTEROS JOHANNA ANAHI</t>
+          <t>BARROJO FEDERICO ALEJANDRO</t>
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>606210</v>
+        <v>606507</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="E12" s="2" t="inlineStr">
         <is>
-          <t>15:30 - 20:00</t>
+          <t>18:00 - 20:00</t>
         </is>
       </c>
       <c r="F12" s="2" t="n">
@@ -929,7 +781,7 @@
       </c>
       <c r="G12" s="2" t="inlineStr">
         <is>
-          <t>VMAJOCAN</t>
+          <t>VMAFEBAR</t>
         </is>
       </c>
       <c r="H12" s="2" t="inlineStr">
@@ -946,18 +798,18 @@
       </c>
       <c r="B13" s="5" t="inlineStr">
         <is>
-          <t>CASTILLO CUEVA LUCIANA</t>
+          <t>BELCHIOR MEDINACELLI LUZ MARIA</t>
         </is>
       </c>
       <c r="C13" s="5" t="n">
-        <v>605901</v>
+        <v>606408</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E13" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 17:30</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F13" s="2" t="n">
@@ -965,12 +817,12 @@
       </c>
       <c r="G13" s="2" t="inlineStr">
         <is>
-          <t>VMALUCCA</t>
+          <t>VMALUBEL</t>
         </is>
       </c>
       <c r="H13" s="2" t="inlineStr">
         <is>
-          <t>GOYECHEA, AGUSTINA LOURDES</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -982,18 +834,18 @@
       </c>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>CASTRO CRISTIAN NICOLAS</t>
+          <t>BERTUCCI AGOSTINA</t>
         </is>
       </c>
       <c r="C14" s="5" t="n">
-        <v>605774</v>
+        <v>605591</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F14" s="2" t="n">
@@ -1001,12 +853,12 @@
       </c>
       <c r="G14" s="2" t="inlineStr">
         <is>
-          <t>VMACRCAS</t>
+          <t>vmaagber</t>
         </is>
       </c>
       <c r="H14" s="2" t="inlineStr">
         <is>
-          <t>SOLER, SANTIAGO MAXIMILIANO</t>
+          <t>ROBLEDO, YESICA DANIELA</t>
         </is>
       </c>
     </row>
@@ -1018,18 +870,18 @@
       </c>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>CEJAS MAYRA</t>
+          <t>BURSESE MAITE PILAR</t>
         </is>
       </c>
       <c r="C15" s="5" t="n">
-        <v>606031</v>
+        <v>606443</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E15" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:30 - 16:00</t>
         </is>
       </c>
       <c r="F15" s="2" t="n">
@@ -1037,12 +889,12 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>VMAMACEJ</t>
+          <t>VMAMABUR</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -1054,18 +906,18 @@
       </c>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>COLMENARES EMILY</t>
+          <t>CALAHUANA SILVANA</t>
         </is>
       </c>
       <c r="C16" s="5" t="n">
-        <v>606645</v>
+        <v>606371</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2" t="inlineStr">
         <is>
-          <t>15:30 - 20:00</t>
+          <t>14:00 - 18:30</t>
         </is>
       </c>
       <c r="F16" s="2" t="n">
@@ -1073,12 +925,12 @@
       </c>
       <c r="G16" s="2" t="inlineStr">
         <is>
-          <t>VMAEMCOL</t>
+          <t>VMASICAL</t>
         </is>
       </c>
       <c r="H16" s="2" t="inlineStr">
         <is>
-          <t>MIR, TOMAS MAURICIO</t>
+          <t>SOLER, SANTIAGO MAXIMILIANO</t>
         </is>
       </c>
     </row>
@@ -1090,18 +942,18 @@
       </c>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>CUBILLA MARLENE ARACELI</t>
+          <t>CANTEROS JOHANNA ANAHI</t>
         </is>
       </c>
       <c r="C17" s="5" t="n">
-        <v>605676</v>
+        <v>606210</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="E17" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 14:30</t>
+          <t>15:30 - 20:00</t>
         </is>
       </c>
       <c r="F17" s="2" t="n">
@@ -1109,12 +961,12 @@
       </c>
       <c r="G17" s="2" t="inlineStr">
         <is>
-          <t>VMAMACUB</t>
+          <t>VMAJOCAN</t>
         </is>
       </c>
       <c r="H17" s="2" t="inlineStr">
         <is>
-          <t>RUIZ, TOMAS EMANUEL</t>
+          <t>MIR, TOMAS MAURICIO</t>
         </is>
       </c>
     </row>
@@ -1126,18 +978,18 @@
       </c>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>DURO CANDELA MILAGROS</t>
+          <t>CASTILLO CUEVA LUCIANA</t>
         </is>
       </c>
       <c r="C18" s="5" t="n">
-        <v>606249</v>
+        <v>605901</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 17:30</t>
         </is>
       </c>
       <c r="F18" s="2" t="n">
@@ -1145,12 +997,12 @@
       </c>
       <c r="G18" s="2" t="inlineStr">
         <is>
-          <t>VMACADUR</t>
+          <t>VMALUCCA</t>
         </is>
       </c>
       <c r="H18" s="2" t="inlineStr">
         <is>
-          <t>GARZON, ROCIO BELEN</t>
+          <t>GOYECHEA, AGUSTINA LOURDES</t>
         </is>
       </c>
     </row>
@@ -1162,18 +1014,18 @@
       </c>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>ESPINOZA CIELO</t>
+          <t>CASTRO CRISTIAN NICOLAS</t>
         </is>
       </c>
       <c r="C19" s="5" t="n">
-        <v>605882</v>
+        <v>605774</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="E19" s="2" t="inlineStr">
         <is>
-          <t>18:00 - 20:00</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F19" s="2" t="n">
@@ -1181,12 +1033,12 @@
       </c>
       <c r="G19" s="2" t="inlineStr">
         <is>
-          <t>VMACIESP</t>
+          <t>VMACRCAS</t>
         </is>
       </c>
       <c r="H19" s="2" t="inlineStr">
         <is>
-          <t>PELOC, MARIA SOLEDAD</t>
+          <t>SOLER, SANTIAGO MAXIMILIANO</t>
         </is>
       </c>
     </row>
@@ -1198,18 +1050,18 @@
       </c>
       <c r="B20" s="5" t="inlineStr">
         <is>
-          <t>FONFRIA VALENTINO</t>
+          <t>CEJAS MAYRA</t>
         </is>
       </c>
       <c r="C20" s="5" t="n">
-        <v>606030</v>
+        <v>606031</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E20" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F20" s="2" t="n">
@@ -1217,12 +1069,12 @@
       </c>
       <c r="G20" s="2" t="inlineStr">
         <is>
-          <t>VMAVAFON</t>
+          <t>VMAMACEJ</t>
         </is>
       </c>
       <c r="H20" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, VICTORIA</t>
+          <t>GOMEZ, SASHA</t>
         </is>
       </c>
     </row>
@@ -1234,18 +1086,18 @@
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>FRAGALE PABLO DANIEL</t>
+          <t>COLMENARES EMILY</t>
         </is>
       </c>
       <c r="C21" s="2" t="n">
-        <v>606558</v>
+        <v>606645</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="E21" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>15:30 - 20:00</t>
         </is>
       </c>
       <c r="F21" s="2" t="n">
@@ -1253,12 +1105,12 @@
       </c>
       <c r="G21" s="2" t="inlineStr">
         <is>
-          <t>VMAPAFRA</t>
+          <t>VMAEMCOL</t>
         </is>
       </c>
       <c r="H21" s="2" t="inlineStr">
         <is>
-          <t>ROBLEDO, YESICA DANIELA</t>
+          <t>MIR, TOMAS MAURICIO</t>
         </is>
       </c>
     </row>
@@ -1270,18 +1122,18 @@
       </c>
       <c r="B22" s="5" t="inlineStr">
         <is>
-          <t>FRIAS BRENDA ANTONELA</t>
+          <t>CUBILLA MARLENE ARACELI</t>
         </is>
       </c>
       <c r="C22" s="5" t="n">
-        <v>605768</v>
+        <v>605676</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:00 - 14:30</t>
         </is>
       </c>
       <c r="F22" s="2" t="n">
@@ -1289,12 +1141,12 @@
       </c>
       <c r="G22" s="2" t="inlineStr">
         <is>
-          <t>VMABRFRI</t>
+          <t>VMAMACUB</t>
         </is>
       </c>
       <c r="H22" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, MAITEN</t>
+          <t>RUIZ, TOMAS EMANUEL</t>
         </is>
       </c>
     </row>
@@ -1306,14 +1158,14 @@
       </c>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>GAYO MATIAS FEDERICO</t>
+          <t>DURO CANDELA MILAGROS</t>
         </is>
       </c>
       <c r="C23" s="5" t="n">
-        <v>606401</v>
+        <v>606249</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E23" s="2" t="inlineStr">
         <is>
@@ -1325,12 +1177,12 @@
       </c>
       <c r="G23" s="2" t="inlineStr">
         <is>
-          <t>VMAMAGAY</t>
+          <t>VMACADUR</t>
         </is>
       </c>
       <c r="H23" s="2" t="inlineStr">
         <is>
-          <t>YBARRA, LUCIA ALDANA</t>
+          <t>GARZON, ROCIO BELEN</t>
         </is>
       </c>
     </row>
@@ -1342,18 +1194,18 @@
       </c>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>GIAVINO ALAN EMMANUEL</t>
+          <t>ESPINOZA CIELO</t>
         </is>
       </c>
       <c r="C24" s="5" t="n">
-        <v>606488</v>
+        <v>605882</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E24" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>18:00 - 20:00</t>
         </is>
       </c>
       <c r="F24" s="2" t="n">
@@ -1361,12 +1213,12 @@
       </c>
       <c r="G24" s="2" t="inlineStr">
         <is>
-          <t>VMAALGIA</t>
+          <t>VMACIESP</t>
         </is>
       </c>
       <c r="H24" s="2" t="inlineStr">
         <is>
-          <t>SORIA, ANA PAULA</t>
+          <t>PELOC, MARIA SOLEDAD</t>
         </is>
       </c>
     </row>
@@ -1378,18 +1230,18 @@
       </c>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>GOMEZ BRUNO NAHUEL</t>
+          <t>FONFRIA VALENTINO</t>
         </is>
       </c>
       <c r="C25" s="5" t="n">
-        <v>606216</v>
+        <v>606030</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E25" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 15:30</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F25" s="2" t="n">
@@ -1397,12 +1249,12 @@
       </c>
       <c r="G25" s="2" t="inlineStr">
         <is>
-          <t>VMABRGOM</t>
+          <t>VMAVAFON</t>
         </is>
       </c>
       <c r="H25" s="2" t="inlineStr">
         <is>
-          <t>ONETTO, MARIA DE LOS MILAGROS</t>
+          <t>VILLALBA, VICTORIA</t>
         </is>
       </c>
     </row>
@@ -1414,18 +1266,18 @@
       </c>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>GOMEZ CESAR NAHUEL</t>
+          <t>FRAGALE PABLO DANIEL</t>
         </is>
       </c>
       <c r="C26" s="5" t="n">
-        <v>606411</v>
+        <v>606558</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="E26" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F26" s="2" t="n">
@@ -1433,12 +1285,12 @@
       </c>
       <c r="G26" s="2" t="inlineStr">
         <is>
-          <t>VMACEGOM</t>
+          <t>VMAPAFRA</t>
         </is>
       </c>
       <c r="H26" s="2" t="inlineStr">
         <is>
-          <t>YBARRA, LUCIA ALDANA</t>
+          <t>ROBLEDO, YESICA DANIELA</t>
         </is>
       </c>
     </row>
@@ -1450,18 +1302,18 @@
       </c>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>GONSALEZ EMILIANO SEBASTIAN</t>
+          <t>FRIAS BRENDA ANTONELA</t>
         </is>
       </c>
       <c r="C27" s="5" t="n">
-        <v>606391</v>
+        <v>605768</v>
       </c>
       <c r="D27" s="2" t="n">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="E27" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 18:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F27" s="2" t="n">
@@ -1469,12 +1321,12 @@
       </c>
       <c r="G27" s="2" t="inlineStr">
         <is>
-          <t>VMAEMGON</t>
+          <t>VMABRFRI</t>
         </is>
       </c>
       <c r="H27" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, AYLEN MILAGROS</t>
+          <t>VILLALBA, MAITEN</t>
         </is>
       </c>
     </row>
@@ -1486,18 +1338,18 @@
       </c>
       <c r="B28" s="5" t="inlineStr">
         <is>
-          <t>GUTIERREZ BRISA CRISTAL</t>
+          <t>GAYO MATIAS FEDERICO</t>
         </is>
       </c>
       <c r="C28" s="5" t="n">
-        <v>606481</v>
+        <v>606401</v>
       </c>
       <c r="D28" s="2" t="n">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="E28" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F28" s="2" t="n">
@@ -1505,12 +1357,12 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>VMABRGUT</t>
+          <t>VMAMAGAY</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, MAITEN</t>
+          <t>YBARRA, LUCIA ALDANA</t>
         </is>
       </c>
     </row>
@@ -1522,18 +1374,18 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>LOPEZ CAROLINA</t>
+          <t>GIAVINO ALAN EMMANUEL</t>
         </is>
       </c>
       <c r="C29" s="2" t="n">
-        <v>606291</v>
+        <v>606488</v>
       </c>
       <c r="D29" s="2" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="E29" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 18:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F29" s="2" t="n">
@@ -1541,12 +1393,12 @@
       </c>
       <c r="G29" s="2" t="inlineStr">
         <is>
-          <t>VMACLOPE</t>
+          <t>VMAALGIA</t>
         </is>
       </c>
       <c r="H29" s="2" t="inlineStr">
         <is>
-          <t>ROBLEDO, LEANDRO JAVIER</t>
+          <t>SORIA, ANA PAULA</t>
         </is>
       </c>
     </row>
@@ -1558,18 +1410,18 @@
       </c>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>MARTINEZ NORBERTO GUSTAVO</t>
+          <t>GOMEZ BRUNO NAHUEL</t>
         </is>
       </c>
       <c r="C30" s="5" t="n">
-        <v>606359</v>
+        <v>606216</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="E30" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>15:00 - 15:30</t>
         </is>
       </c>
       <c r="F30" s="2" t="n">
@@ -1577,12 +1429,12 @@
       </c>
       <c r="G30" s="2" t="inlineStr">
         <is>
-          <t>VMANOMAR</t>
+          <t>VMABRGOM</t>
         </is>
       </c>
       <c r="H30" s="2" t="inlineStr">
         <is>
-          <t>DIAZ, PAULA</t>
+          <t>ONETTO, MARIA DE LOS MILAGROS</t>
         </is>
       </c>
     </row>
@@ -1594,18 +1446,18 @@
       </c>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t>MENDOZA NATALIA ELIZABETH</t>
+          <t>GOMEZ CESAR NAHUEL</t>
         </is>
       </c>
       <c r="C31" s="5" t="n">
-        <v>605511</v>
+        <v>606411</v>
       </c>
       <c r="D31" s="2" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
       <c r="E31" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 14:30</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F31" s="2" t="n">
@@ -1613,12 +1465,12 @@
       </c>
       <c r="G31" s="2" t="inlineStr">
         <is>
-          <t>VMANAMEN</t>
+          <t>VMACEGOM</t>
         </is>
       </c>
       <c r="H31" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, VICTORIA</t>
+          <t>YBARRA, LUCIA ALDANA</t>
         </is>
       </c>
     </row>
@@ -1630,18 +1482,18 @@
       </c>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>MOREAU MICAELA VICTORIA</t>
+          <t>GONSALEZ EMILIANO SEBASTIAN</t>
         </is>
       </c>
       <c r="C32" s="5" t="n">
-        <v>606331</v>
+        <v>606391</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E32" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:30 - 18:00</t>
         </is>
       </c>
       <c r="F32" s="2" t="n">
@@ -1649,12 +1501,12 @@
       </c>
       <c r="G32" s="2" t="inlineStr">
         <is>
-          <t>VMAMIMOR</t>
+          <t>VMAEMGON</t>
         </is>
       </c>
       <c r="H32" s="2" t="inlineStr">
         <is>
-          <t>SOLER, SANTIAGO MAXIMILIANO</t>
+          <t>GOMEZ, AYLEN MILAGROS</t>
         </is>
       </c>
     </row>
@@ -1666,18 +1518,18 @@
       </c>
       <c r="B33" s="5" t="inlineStr">
         <is>
-          <t>MOSQUEIRA HERNAN FEDERICO</t>
+          <t>GUTIERREZ BRISA CRISTAL</t>
         </is>
       </c>
       <c r="C33" s="5" t="n">
-        <v>606306</v>
+        <v>606481</v>
       </c>
       <c r="D33" s="2" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F33" s="2" t="n">
@@ -1685,12 +1537,12 @@
       </c>
       <c r="G33" s="2" t="inlineStr">
         <is>
-          <t>VMAFEMOS</t>
+          <t>VMABRGUT</t>
         </is>
       </c>
       <c r="H33" s="2" t="inlineStr">
         <is>
-          <t>DIAZ, PAULA</t>
+          <t>VILLALBA, MAITEN</t>
         </is>
       </c>
     </row>
@@ -1702,18 +1554,18 @@
       </c>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>NARBONA SUSAN ABRIL</t>
+          <t>LOPEZ CAROLINA</t>
         </is>
       </c>
       <c r="C34" s="5" t="n">
-        <v>606227</v>
+        <v>606291</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="E34" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 18:00</t>
         </is>
       </c>
       <c r="F34" s="2" t="n">
@@ -1721,12 +1573,12 @@
       </c>
       <c r="G34" s="2" t="inlineStr">
         <is>
-          <t>VMASUNAR</t>
+          <t>VMACLOPE</t>
         </is>
       </c>
       <c r="H34" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, MAITEN</t>
+          <t>ROBLEDO, LEANDRO JAVIER</t>
         </is>
       </c>
     </row>
@@ -1738,18 +1590,18 @@
       </c>
       <c r="B35" s="5" t="inlineStr">
         <is>
-          <t>QUISBERT ARUATA ANDREW ROBERT</t>
+          <t>MARTINEZ NORBERTO GUSTAVO</t>
         </is>
       </c>
       <c r="C35" s="5" t="n">
-        <v>606478</v>
+        <v>606359</v>
       </c>
       <c r="D35" s="2" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="E35" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F35" s="2" t="n">
@@ -1757,7 +1609,7 @@
       </c>
       <c r="G35" s="2" t="inlineStr">
         <is>
-          <t>VMAANQUI</t>
+          <t>VMANOMAR</t>
         </is>
       </c>
       <c r="H35" s="2" t="inlineStr">
@@ -1774,18 +1626,18 @@
       </c>
       <c r="B36" s="5" t="inlineStr">
         <is>
-          <t>RIQUELME LUCIA</t>
+          <t>MENDOZA NATALIA ELIZABETH</t>
         </is>
       </c>
       <c r="C36" s="5" t="n">
-        <v>606577</v>
+        <v>605511</v>
       </c>
       <c r="D36" s="2" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E36" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 14:30</t>
         </is>
       </c>
       <c r="F36" s="2" t="n">
@@ -1793,12 +1645,12 @@
       </c>
       <c r="G36" s="2" t="inlineStr">
         <is>
-          <t>VMALURIQ</t>
+          <t>VMANAMEN</t>
         </is>
       </c>
       <c r="H36" s="2" t="inlineStr">
         <is>
-          <t>LOUREIRO, FLORENCIA CANDELA</t>
+          <t>VILLALBA, VICTORIA</t>
         </is>
       </c>
     </row>
@@ -1810,18 +1662,18 @@
       </c>
       <c r="B37" s="5" t="inlineStr">
         <is>
-          <t>ROLON NANCY MAGALI</t>
+          <t>MOREAU MICAELA VICTORIA</t>
         </is>
       </c>
       <c r="C37" s="5" t="n">
-        <v>606550</v>
+        <v>606331</v>
       </c>
       <c r="D37" s="2" t="n">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E37" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F37" s="2" t="n">
@@ -1829,12 +1681,12 @@
       </c>
       <c r="G37" s="2" t="inlineStr">
         <is>
-          <t>VMANAROL</t>
+          <t>VMAMIMOR</t>
         </is>
       </c>
       <c r="H37" s="2" t="inlineStr">
         <is>
-          <t>GROESMANN, MAYA JUDITH</t>
+          <t>SOLER, SANTIAGO MAXIMILIANO</t>
         </is>
       </c>
     </row>
@@ -1846,18 +1698,18 @@
       </c>
       <c r="B38" s="5" t="inlineStr">
         <is>
-          <t>ROMITO AGOSTINA BELEN</t>
+          <t>MOSQUEIRA HERNAN FEDERICO</t>
         </is>
       </c>
       <c r="C38" s="5" t="n">
-        <v>606286</v>
+        <v>606306</v>
       </c>
       <c r="D38" s="2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E38" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 16:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F38" s="2" t="n">
@@ -1865,12 +1717,12 @@
       </c>
       <c r="G38" s="2" t="inlineStr">
         <is>
-          <t>VMAAGROM</t>
+          <t>VMAFEMOS</t>
         </is>
       </c>
       <c r="H38" s="2" t="inlineStr">
         <is>
-          <t>ONETTO, MARIA DE LOS MILAGROS</t>
+          <t>DIAZ, PAULA</t>
         </is>
       </c>
     </row>
@@ -1882,18 +1734,18 @@
       </c>
       <c r="B39" s="5" t="inlineStr">
         <is>
-          <t>SANJUAN LAURA</t>
+          <t>NARBONA SUSAN ABRIL</t>
         </is>
       </c>
       <c r="C39" s="5" t="n">
-        <v>606436</v>
+        <v>606227</v>
       </c>
       <c r="D39" s="2" t="n">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F39" s="2" t="n">
@@ -1901,12 +1753,12 @@
       </c>
       <c r="G39" s="2" t="inlineStr">
         <is>
-          <t>VMALASAN</t>
+          <t>VMASUNAR</t>
         </is>
       </c>
       <c r="H39" s="2" t="inlineStr">
         <is>
-          <t>ROJAS, LUCAS</t>
+          <t>VILLALBA, MAITEN</t>
         </is>
       </c>
     </row>
@@ -1918,18 +1770,18 @@
       </c>
       <c r="B40" s="5" t="inlineStr">
         <is>
-          <t>SANSO NOEMI</t>
+          <t>QUISBERT ARUATA ANDREW ROBERT</t>
         </is>
       </c>
       <c r="C40" s="5" t="n">
-        <v>606492</v>
+        <v>606478</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="E40" s="2" t="inlineStr">
         <is>
-          <t>17:30 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F40" s="2" t="n">
@@ -1937,12 +1789,12 @@
       </c>
       <c r="G40" s="2" t="inlineStr">
         <is>
-          <t>VMANASAN</t>
+          <t>VMAANQUI</t>
         </is>
       </c>
       <c r="H40" s="2" t="inlineStr">
         <is>
-          <t>MIR, TOMAS MAURICIO</t>
+          <t>DIAZ, PAULA</t>
         </is>
       </c>
     </row>
@@ -1954,18 +1806,18 @@
       </c>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t>SOLIS MELINA ALEJANDRA</t>
+          <t>RIQUELME LUCIA</t>
         </is>
       </c>
       <c r="C41" s="5" t="n">
-        <v>605698</v>
+        <v>606577</v>
       </c>
       <c r="D41" s="2" t="n">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="E41" s="2" t="inlineStr">
         <is>
-          <t>15:30 - 20:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F41" s="2" t="n">
@@ -1973,12 +1825,12 @@
       </c>
       <c r="G41" s="2" t="inlineStr">
         <is>
-          <t>VMAMELSO</t>
+          <t>VMALURIQ</t>
         </is>
       </c>
       <c r="H41" s="2" t="inlineStr">
         <is>
-          <t>PELOC, MARIA SOLEDAD</t>
+          <t>LOUREIRO, FLORENCIA CANDELA</t>
         </is>
       </c>
     </row>
@@ -1990,18 +1842,18 @@
       </c>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>SOSA BERNAO MARTINA</t>
+          <t>ROLON NANCY MAGALI</t>
         </is>
       </c>
       <c r="C42" s="5" t="n">
-        <v>606614</v>
+        <v>606550</v>
       </c>
       <c r="D42" s="2" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E42" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F42" s="2" t="n">
@@ -2009,12 +1861,12 @@
       </c>
       <c r="G42" s="2" t="inlineStr">
         <is>
-          <t>VMAMARSO</t>
+          <t>VMANAROL</t>
         </is>
       </c>
       <c r="H42" s="2" t="inlineStr">
         <is>
-          <t>GARZON, ROCIO BELEN</t>
+          <t>GROESMANN, MAYA JUDITH</t>
         </is>
       </c>
     </row>
@@ -2026,18 +1878,18 @@
       </c>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>SOTELO SILVANA ANAHI</t>
+          <t>ROMITO AGOSTINA BELEN</t>
         </is>
       </c>
       <c r="C43" s="5" t="n">
-        <v>606536</v>
+        <v>606286</v>
       </c>
       <c r="D43" s="2" t="n">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="E43" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>15:00 - 16:00</t>
         </is>
       </c>
       <c r="F43" s="2" t="n">
@@ -2045,12 +1897,12 @@
       </c>
       <c r="G43" s="2" t="inlineStr">
         <is>
-          <t>VMASISOT</t>
+          <t>VMAAGROM</t>
         </is>
       </c>
       <c r="H43" s="2" t="inlineStr">
         <is>
-          <t>SOLER, SANTIAGO MAXIMILIANO</t>
+          <t>ONETTO, MARIA DE LOS MILAGROS</t>
         </is>
       </c>
     </row>
@@ -2062,18 +1914,18 @@
       </c>
       <c r="B44" s="5" t="inlineStr">
         <is>
-          <t>TOFFOLETTI SOTO EVELYN</t>
+          <t>SANJUAN LAURA</t>
         </is>
       </c>
       <c r="C44" s="5" t="n">
-        <v>606501</v>
+        <v>606436</v>
       </c>
       <c r="D44" s="2" t="n">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="E44" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F44" s="2" t="n">
@@ -2081,12 +1933,12 @@
       </c>
       <c r="G44" s="2" t="inlineStr">
         <is>
-          <t>VMAEVTOF</t>
+          <t>VMALASAN</t>
         </is>
       </c>
       <c r="H44" s="2" t="inlineStr">
         <is>
-          <t>GROESMANN, MAYA JUDITH</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -2098,18 +1950,18 @@
       </c>
       <c r="B45" s="5" t="inlineStr">
         <is>
-          <t>TOLOZA ESTEFANIA KAREN</t>
+          <t>SANSO NOEMI</t>
         </is>
       </c>
       <c r="C45" s="5" t="n">
-        <v>605508</v>
+        <v>606492</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E45" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 20:00</t>
+          <t>17:30 - 20:00</t>
         </is>
       </c>
       <c r="F45" s="2" t="n">
@@ -2117,12 +1969,12 @@
       </c>
       <c r="G45" s="2" t="inlineStr">
         <is>
-          <t>VMAESTOL</t>
+          <t>VMANASAN</t>
         </is>
       </c>
       <c r="H45" s="2" t="inlineStr">
         <is>
-          <t>DIAZ, PAULA</t>
+          <t>MIR, TOMAS MAURICIO</t>
         </is>
       </c>
     </row>
@@ -2134,18 +1986,18 @@
       </c>
       <c r="B46" s="5" t="inlineStr">
         <is>
-          <t>TORRES LUNA</t>
+          <t>SOLIS MELINA ALEJANDRA</t>
         </is>
       </c>
       <c r="C46" s="5" t="n">
-        <v>606239</v>
+        <v>605698</v>
       </c>
       <c r="D46" s="2" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="E46" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>15:30 - 20:00</t>
         </is>
       </c>
       <c r="F46" s="2" t="n">
@@ -2153,12 +2005,12 @@
       </c>
       <c r="G46" s="2" t="inlineStr">
         <is>
-          <t>VMALUTOR</t>
+          <t>VMAMELSO</t>
         </is>
       </c>
       <c r="H46" s="2" t="inlineStr">
         <is>
-          <t>RUIZ, TOMAS EMANUEL</t>
+          <t>PELOC, MARIA SOLEDAD</t>
         </is>
       </c>
     </row>
@@ -2170,18 +2022,18 @@
       </c>
       <c r="B47" s="5" t="inlineStr">
         <is>
-          <t>VACA OROZCO ANDREA</t>
+          <t>SOSA BERNAO MARTINA</t>
         </is>
       </c>
       <c r="C47" s="5" t="n">
-        <v>606475</v>
+        <v>606614</v>
       </c>
       <c r="D47" s="2" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="E47" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:30</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F47" s="2" t="n">
@@ -2189,12 +2041,12 @@
       </c>
       <c r="G47" s="2" t="inlineStr">
         <is>
-          <t>VMAANVAC</t>
+          <t>VMAMARSO</t>
         </is>
       </c>
       <c r="H47" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, MAITEN</t>
+          <t>GARZON, ROCIO BELEN</t>
         </is>
       </c>
     </row>
@@ -2206,14 +2058,14 @@
       </c>
       <c r="B48" s="5" t="inlineStr">
         <is>
-          <t>ZAPATA VAGNINI MARTINA</t>
+          <t>SOTELO SILVANA ANAHI</t>
         </is>
       </c>
       <c r="C48" s="5" t="n">
-        <v>605766</v>
+        <v>606536</v>
       </c>
       <c r="D48" s="2" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E48" s="2" t="inlineStr">
         <is>
@@ -2225,7 +2077,7 @@
       </c>
       <c r="G48" s="2" t="inlineStr">
         <is>
-          <t>VMAMAZAP</t>
+          <t>VMASISOT</t>
         </is>
       </c>
       <c r="H48" s="2" t="inlineStr">
@@ -2242,18 +2094,18 @@
       </c>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>RUSSO ROCIO BELEN</t>
+          <t>TOFFOLETTI SOTO EVELYN</t>
         </is>
       </c>
       <c r="C49" s="5" t="n">
-        <v>605503</v>
+        <v>606501</v>
       </c>
       <c r="D49" s="2" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E49" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F49" s="2" t="n">
@@ -2261,12 +2113,12 @@
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
-          <t>VMARORUS</t>
+          <t>VMAEVTOF</t>
         </is>
       </c>
       <c r="H49" s="2" t="inlineStr">
         <is>
-          <t>ROBLEDO, YESICA DANIELA</t>
+          <t>GROESMANN, MAYA JUDITH</t>
         </is>
       </c>
     </row>
@@ -2278,18 +2130,18 @@
       </c>
       <c r="B50" s="5" t="inlineStr">
         <is>
-          <t>WETZEL IGNACIO EZEQUIEL</t>
+          <t>TOLOZA ESTEFANIA KAREN</t>
         </is>
       </c>
       <c r="C50" s="5" t="n">
-        <v>605982</v>
+        <v>605508</v>
       </c>
       <c r="D50" s="2" t="n">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="E50" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:00 - 20:00</t>
         </is>
       </c>
       <c r="F50" s="2" t="n">
@@ -2297,35 +2149,35 @@
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
-          <t>VMAIGWET</t>
+          <t>VMAESTOL</t>
         </is>
       </c>
       <c r="H50" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, VICTORIA</t>
+          <t>DIAZ, PAULA</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="inlineStr">
         <is>
-          <t>S2S PREMIUM</t>
+          <t>S2S NO PREMIUM</t>
         </is>
       </c>
       <c r="B51" s="5" t="inlineStr">
         <is>
-          <t>ABALOS HEREDIA DAIANA BELEN</t>
+          <t>TORRES LUNA</t>
         </is>
       </c>
       <c r="C51" s="5" t="n">
-        <v>606348</v>
+        <v>606239</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>37</v>
+        <v>4</v>
       </c>
       <c r="E51" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F51" s="2" t="n">
@@ -2333,35 +2185,35 @@
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>VMADAABA</t>
+          <t>VMALUTOR</t>
         </is>
       </c>
       <c r="H51" s="2" t="inlineStr">
         <is>
-          <t>ROJAS, LUCAS</t>
+          <t>RUIZ, TOMAS EMANUEL</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="inlineStr">
         <is>
-          <t>S2S PREMIUM</t>
+          <t>S2S NO PREMIUM</t>
         </is>
       </c>
       <c r="B52" s="5" t="inlineStr">
         <is>
-          <t>BENITEZ LOURDES ROCIO</t>
+          <t>VACA OROZCO ANDREA</t>
         </is>
       </c>
       <c r="C52" s="5" t="n">
-        <v>605986</v>
+        <v>606475</v>
       </c>
       <c r="D52" s="2" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
-          <t>18:00 - 18:30</t>
+          <t>14:00 - 16:30</t>
         </is>
       </c>
       <c r="F52" s="2" t="n">
@@ -2369,35 +2221,35 @@
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
-          <t>VMALOBEN</t>
+          <t>VMAANVAC</t>
         </is>
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>YBARRA, LUCIA ALDANA</t>
+          <t>VILLALBA, MAITEN</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>S2S PREMIUM</t>
+          <t>S2S NO PREMIUM</t>
         </is>
       </c>
       <c r="B53" s="5" t="inlineStr">
         <is>
-          <t>CASTILLO MICAELA TATIANA</t>
+          <t>ZAPATA VAGNINI MARTINA</t>
         </is>
       </c>
       <c r="C53" s="5" t="n">
-        <v>605589</v>
+        <v>605766</v>
       </c>
       <c r="D53" s="2" t="n">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="E53" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 17:30</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F53" s="2" t="n">
@@ -2405,35 +2257,35 @@
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>VMAMICCA</t>
+          <t>VMAMAZAP</t>
         </is>
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>SOLER, SANTIAGO MAXIMILIANO</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>S2S PREMIUM</t>
+          <t>S2S NO PREMIUM</t>
         </is>
       </c>
       <c r="B54" s="5" t="inlineStr">
         <is>
-          <t>CERVANTES LOURDES ABRIL</t>
+          <t>RUSSO ROCIO BELEN</t>
         </is>
       </c>
       <c r="C54" s="5" t="n">
-        <v>606528</v>
+        <v>605503</v>
       </c>
       <c r="D54" s="2" t="n">
-        <v>44</v>
+        <v>11</v>
       </c>
       <c r="E54" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 20:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F54" s="2" t="n">
@@ -2441,35 +2293,35 @@
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
-          <t>VMALOCER</t>
+          <t>VMARORUS</t>
         </is>
       </c>
       <c r="H54" s="2" t="inlineStr">
         <is>
-          <t>YBARRA, LUCIA ALDANA</t>
+          <t>ROBLEDO, YESICA DANIELA</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>S2S PREMIUM</t>
+          <t>S2S NO PREMIUM</t>
         </is>
       </c>
       <c r="B55" s="5" t="inlineStr">
         <is>
-          <t>CORIA CANDELA</t>
+          <t>WETZEL IGNACIO EZEQUIEL</t>
         </is>
       </c>
       <c r="C55" s="5" t="n">
-        <v>606623</v>
+        <v>605982</v>
       </c>
       <c r="D55" s="2" t="n">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="E55" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 20:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F55" s="2" t="n">
@@ -2477,12 +2329,12 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>VMACANCO</t>
+          <t>VMAIGWET</t>
         </is>
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>GARZON, ROCIO BELEN</t>
+          <t>VILLALBA, VICTORIA</t>
         </is>
       </c>
     </row>
@@ -2494,18 +2346,18 @@
       </c>
       <c r="B56" s="5" t="inlineStr">
         <is>
-          <t>CUELLAR JOEL ADRIAN</t>
+          <t>ABALOS HEREDIA DAIANA BELEN</t>
         </is>
       </c>
       <c r="C56" s="5" t="n">
-        <v>605760</v>
+        <v>606348</v>
       </c>
       <c r="D56" s="2" t="n">
-        <v>7</v>
+        <v>37</v>
       </c>
       <c r="E56" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F56" s="2" t="n">
@@ -2513,12 +2365,12 @@
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
-          <t>VMAJOCUE</t>
+          <t>VMADAABA</t>
         </is>
       </c>
       <c r="H56" s="2" t="inlineStr">
         <is>
-          <t>LOUREIRO, FLORENCIA CANDELA</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -2530,18 +2382,18 @@
       </c>
       <c r="B57" s="5" t="inlineStr">
         <is>
-          <t>D AGOSTINO MARIA BIANCA</t>
+          <t>BENITEZ LOURDES ROCIO</t>
         </is>
       </c>
       <c r="C57" s="5" t="n">
-        <v>605611</v>
+        <v>605986</v>
       </c>
       <c r="D57" s="2" t="n">
-        <v>38</v>
+        <v>1</v>
       </c>
       <c r="E57" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 20:00</t>
+          <t>18:00 - 18:30</t>
         </is>
       </c>
       <c r="F57" s="2" t="n">
@@ -2549,7 +2401,7 @@
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>VMAMADAG</t>
+          <t>VMALOBEN</t>
         </is>
       </c>
       <c r="H57" s="2" t="inlineStr">
@@ -2566,18 +2418,18 @@
       </c>
       <c r="B58" s="5" t="inlineStr">
         <is>
-          <t>DE VUONO FACUNDO SANTIAGO</t>
+          <t>CASTILLO MICAELA TATIANA</t>
         </is>
       </c>
       <c r="C58" s="5" t="n">
-        <v>605617</v>
+        <v>605589</v>
       </c>
       <c r="D58" s="2" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E58" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 17:30</t>
+          <t>14:30 - 17:30</t>
         </is>
       </c>
       <c r="F58" s="2" t="n">
@@ -2585,7 +2437,7 @@
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>VMAFACDE</t>
+          <t>VMAMICCA</t>
         </is>
       </c>
       <c r="H58" s="2" t="inlineStr">
@@ -2602,18 +2454,18 @@
       </c>
       <c r="B59" s="5" t="inlineStr">
         <is>
-          <t>DEMARCO FIDEL</t>
+          <t>CERVANTES LOURDES ABRIL</t>
         </is>
       </c>
       <c r="C59" s="5" t="n">
-        <v>605969</v>
+        <v>606528</v>
       </c>
       <c r="D59" s="2" t="n">
-        <v>8</v>
+        <v>44</v>
       </c>
       <c r="E59" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>14:00 - 20:00</t>
         </is>
       </c>
       <c r="F59" s="2" t="n">
@@ -2621,12 +2473,12 @@
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
-          <t>VMAFIDEM</t>
+          <t>VMALOCER</t>
         </is>
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, VICTORIA</t>
+          <t>YBARRA, LUCIA ALDANA</t>
         </is>
       </c>
     </row>
@@ -2638,18 +2490,18 @@
       </c>
       <c r="B60" s="5" t="inlineStr">
         <is>
-          <t>DONZELLI ANGELICA</t>
+          <t>CORIA CANDELA</t>
         </is>
       </c>
       <c r="C60" s="5" t="n">
-        <v>606309</v>
+        <v>606623</v>
       </c>
       <c r="D60" s="2" t="n">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="E60" s="2" t="inlineStr">
         <is>
-          <t>18:30 - 20:00</t>
+          <t>14:00 - 20:00</t>
         </is>
       </c>
       <c r="F60" s="2" t="n">
@@ -2657,12 +2509,12 @@
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>VMAANDON</t>
+          <t>VMACANCO</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>ROBLEDO, LEANDRO JAVIER</t>
+          <t>GARZON, ROCIO BELEN</t>
         </is>
       </c>
     </row>
@@ -2674,18 +2526,18 @@
       </c>
       <c r="B61" s="5" t="inlineStr">
         <is>
-          <t>FERREYRA TOMAS AGUSTIN</t>
+          <t>CUELLAR JOEL ADRIAN</t>
         </is>
       </c>
       <c r="C61" s="5" t="n">
-        <v>605580</v>
+        <v>605760</v>
       </c>
       <c r="D61" s="2" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E61" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F61" s="2" t="n">
@@ -2693,12 +2545,12 @@
       </c>
       <c r="G61" s="2" t="inlineStr">
         <is>
-          <t>VMATOFER</t>
+          <t>VMAJOCUE</t>
         </is>
       </c>
       <c r="H61" s="2" t="inlineStr">
         <is>
-          <t>GROESMANN, MAYA JUDITH</t>
+          <t>LOUREIRO, FLORENCIA CANDELA</t>
         </is>
       </c>
     </row>
@@ -2710,18 +2562,18 @@
       </c>
       <c r="B62" s="5" t="inlineStr">
         <is>
-          <t>FRAGA NICOLAS</t>
+          <t>D AGOSTINO MARIA BIANCA</t>
         </is>
       </c>
       <c r="C62" s="5" t="n">
-        <v>605763</v>
+        <v>605611</v>
       </c>
       <c r="D62" s="2" t="n">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E62" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 17:30</t>
+          <t>14:00 - 20:00</t>
         </is>
       </c>
       <c r="F62" s="2" t="n">
@@ -2729,12 +2581,12 @@
       </c>
       <c r="G62" s="2" t="inlineStr">
         <is>
-          <t>VMANIFRA</t>
+          <t>VMAMADAG</t>
         </is>
       </c>
       <c r="H62" s="2" t="inlineStr">
         <is>
-          <t>ROJAS, LUCAS</t>
+          <t>YBARRA, LUCIA ALDANA</t>
         </is>
       </c>
     </row>
@@ -2746,18 +2598,18 @@
       </c>
       <c r="B63" s="5" t="inlineStr">
         <is>
-          <t>FRANCO SELENA ROCIO</t>
+          <t>DE VUONO FACUNDO SANTIAGO</t>
         </is>
       </c>
       <c r="C63" s="5" t="n">
-        <v>606330</v>
+        <v>605617</v>
       </c>
       <c r="D63" s="2" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="E63" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>15:00 - 17:30</t>
         </is>
       </c>
       <c r="F63" s="2" t="n">
@@ -2765,12 +2617,12 @@
       </c>
       <c r="G63" s="2" t="inlineStr">
         <is>
-          <t>VMASEFRA</t>
+          <t>VMAFACDE</t>
         </is>
       </c>
       <c r="H63" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, AYLEN MILAGROS</t>
+          <t>GOMEZ, SASHA</t>
         </is>
       </c>
     </row>
@@ -2782,18 +2634,18 @@
       </c>
       <c r="B64" s="5" t="inlineStr">
         <is>
-          <t>FUHR PATRICIO ALEJANDRO</t>
+          <t>DEMARCO FIDEL</t>
         </is>
       </c>
       <c r="C64" s="5" t="n">
-        <v>606457</v>
+        <v>605969</v>
       </c>
       <c r="D64" s="2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E64" s="2" t="inlineStr">
         <is>
-          <t>18:00 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F64" s="2" t="n">
@@ -2801,12 +2653,12 @@
       </c>
       <c r="G64" s="2" t="inlineStr">
         <is>
-          <t>VMAPAFUH</t>
+          <t>VMAFIDEM</t>
         </is>
       </c>
       <c r="H64" s="2" t="inlineStr">
         <is>
-          <t>MIR, TOMAS MAURICIO</t>
+          <t>VILLALBA, VICTORIA</t>
         </is>
       </c>
     </row>
@@ -2818,18 +2670,18 @@
       </c>
       <c r="B65" s="5" t="inlineStr">
         <is>
-          <t>GARRIGO CAROLINA</t>
+          <t>DONZELLI ANGELICA</t>
         </is>
       </c>
       <c r="C65" s="5" t="n">
-        <v>606445</v>
+        <v>606309</v>
       </c>
       <c r="D65" s="2" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E65" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>18:30 - 20:00</t>
         </is>
       </c>
       <c r="F65" s="2" t="n">
@@ -2837,12 +2689,12 @@
       </c>
       <c r="G65" s="2" t="inlineStr">
         <is>
-          <t>VMACAGAR</t>
+          <t>VMAANDON</t>
         </is>
       </c>
       <c r="H65" s="2" t="inlineStr">
         <is>
-          <t>DIAZ, PAULA</t>
+          <t>ROBLEDO, LEANDRO JAVIER</t>
         </is>
       </c>
     </row>
@@ -2854,18 +2706,18 @@
       </c>
       <c r="B66" s="5" t="inlineStr">
         <is>
-          <t>GOMEZ ENCISO MONICA</t>
+          <t>FERREYRA TOMAS AGUSTIN</t>
         </is>
       </c>
       <c r="C66" s="5" t="n">
-        <v>606039</v>
+        <v>605580</v>
       </c>
       <c r="D66" s="2" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="E66" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F66" s="2" t="n">
@@ -2873,12 +2725,12 @@
       </c>
       <c r="G66" s="2" t="inlineStr">
         <is>
-          <t>VMAMOGOM</t>
+          <t>VMATOFER</t>
         </is>
       </c>
       <c r="H66" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>GROESMANN, MAYA JUDITH</t>
         </is>
       </c>
     </row>
@@ -2890,18 +2742,18 @@
       </c>
       <c r="B67" s="5" t="inlineStr">
         <is>
-          <t>GONZALEZ CANDELA</t>
+          <t>FRAGA NICOLAS</t>
         </is>
       </c>
       <c r="C67" s="5" t="n">
-        <v>605826</v>
+        <v>605763</v>
       </c>
       <c r="D67" s="2" t="n">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E67" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>14:00 - 17:30</t>
         </is>
       </c>
       <c r="F67" s="2" t="n">
@@ -2909,12 +2761,12 @@
       </c>
       <c r="G67" s="2" t="inlineStr">
         <is>
-          <t>VMACAGON</t>
+          <t>VMANIFRA</t>
         </is>
       </c>
       <c r="H67" s="2" t="inlineStr">
         <is>
-          <t>GROESMANN, MAYA JUDITH</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -2926,18 +2778,18 @@
       </c>
       <c r="B68" s="5" t="inlineStr">
         <is>
-          <t>GONZALEZ CRISTIAN ALBERTO</t>
+          <t>FRANCO SELENA ROCIO</t>
         </is>
       </c>
       <c r="C68" s="5" t="n">
-        <v>606338</v>
+        <v>606330</v>
       </c>
       <c r="D68" s="2" t="n">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E68" s="2" t="inlineStr">
         <is>
-          <t>17:30 - 20:00</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F68" s="2" t="n">
@@ -2945,12 +2797,12 @@
       </c>
       <c r="G68" s="2" t="inlineStr">
         <is>
-          <t>VMACRGON</t>
+          <t>VMASEFRA</t>
         </is>
       </c>
       <c r="H68" s="2" t="inlineStr">
         <is>
-          <t>ROJAS, LUCAS</t>
+          <t>GOMEZ, AYLEN MILAGROS</t>
         </is>
       </c>
     </row>
@@ -2962,18 +2814,18 @@
       </c>
       <c r="B69" s="5" t="inlineStr">
         <is>
-          <t>INFANTE ENZO</t>
+          <t>FUHR PATRICIO ALEJANDRO</t>
         </is>
       </c>
       <c r="C69" s="5" t="n">
-        <v>605911</v>
+        <v>606457</v>
       </c>
       <c r="D69" s="2" t="n">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E69" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>18:00 - 20:00</t>
         </is>
       </c>
       <c r="F69" s="2" t="n">
@@ -2981,12 +2833,12 @@
       </c>
       <c r="G69" s="2" t="inlineStr">
         <is>
-          <t>VMAENINF</t>
+          <t>VMAPAFUH</t>
         </is>
       </c>
       <c r="H69" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, AYLEN MILAGROS</t>
+          <t>MIR, TOMAS MAURICIO</t>
         </is>
       </c>
     </row>
@@ -2998,18 +2850,18 @@
       </c>
       <c r="B70" s="5" t="inlineStr">
         <is>
-          <t>MACHADO RIVERA ELIAS RAUL</t>
+          <t>GARRIGO CAROLINA</t>
         </is>
       </c>
       <c r="C70" s="5" t="n">
-        <v>606463</v>
+        <v>606445</v>
       </c>
       <c r="D70" s="2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E70" s="2" t="inlineStr">
         <is>
-          <t>19:30 - 20:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F70" s="2" t="n">
@@ -3017,12 +2869,12 @@
       </c>
       <c r="G70" s="2" t="inlineStr">
         <is>
-          <t>VMAELMAC</t>
+          <t>VMACAGAR</t>
         </is>
       </c>
       <c r="H70" s="2" t="inlineStr">
         <is>
-          <t>GOYECHEA, AGUSTINA LOURDES</t>
+          <t>DIAZ, PAULA</t>
         </is>
       </c>
     </row>
@@ -3034,18 +2886,18 @@
       </c>
       <c r="B71" s="5" t="inlineStr">
         <is>
-          <t>MAIDANA MENDOZA MALENA MELISA</t>
+          <t>GOMEZ ENCISO MONICA</t>
         </is>
       </c>
       <c r="C71" s="5" t="n">
-        <v>605513</v>
+        <v>606039</v>
       </c>
       <c r="D71" s="2" t="n">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="E71" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 18:00</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F71" s="2" t="n">
@@ -3053,12 +2905,12 @@
       </c>
       <c r="G71" s="2" t="inlineStr">
         <is>
-          <t>VMAMAMAI</t>
+          <t>VMAMOGOM</t>
         </is>
       </c>
       <c r="H71" s="2" t="inlineStr">
         <is>
-          <t>YBARRA, LUCIA ALDANA</t>
+          <t>GOMEZ, SASHA</t>
         </is>
       </c>
     </row>
@@ -3070,18 +2922,18 @@
       </c>
       <c r="B72" s="5" t="inlineStr">
         <is>
-          <t>MAIZ CAMILA</t>
+          <t>GONZALEZ CANDELA</t>
         </is>
       </c>
       <c r="C72" s="5" t="n">
-        <v>606219</v>
+        <v>605826</v>
       </c>
       <c r="D72" s="2" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E72" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F72" s="2" t="n">
@@ -3089,12 +2941,12 @@
       </c>
       <c r="G72" s="2" t="inlineStr">
         <is>
-          <t>VMACAMAI</t>
+          <t>VMACAGON</t>
         </is>
       </c>
       <c r="H72" s="2" t="inlineStr">
         <is>
-          <t>ONETTO, MARIA DE LOS MILAGROS</t>
+          <t>GROESMANN, MAYA JUDITH</t>
         </is>
       </c>
     </row>
@@ -3106,18 +2958,18 @@
       </c>
       <c r="B73" s="5" t="inlineStr">
         <is>
-          <t>MANFREDI RUTH MELINA</t>
+          <t>GONZALEZ CRISTIAN ALBERTO</t>
         </is>
       </c>
       <c r="C73" s="5" t="n">
-        <v>605632</v>
+        <v>606338</v>
       </c>
       <c r="D73" s="2" t="n">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="E73" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>17:30 - 20:00</t>
         </is>
       </c>
       <c r="F73" s="2" t="n">
@@ -3125,12 +2977,12 @@
       </c>
       <c r="G73" s="2" t="inlineStr">
         <is>
-          <t>VMAMEMAN</t>
+          <t>VMACRGON</t>
         </is>
       </c>
       <c r="H73" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -3142,18 +2994,18 @@
       </c>
       <c r="B74" s="5" t="inlineStr">
         <is>
-          <t>MARAZ AYELEN JACQUELINE</t>
+          <t>INFANTE ENZO</t>
         </is>
       </c>
       <c r="C74" s="5" t="n">
-        <v>606142</v>
+        <v>605911</v>
       </c>
       <c r="D74" s="2" t="n">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="E74" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F74" s="2" t="n">
@@ -3161,12 +3013,12 @@
       </c>
       <c r="G74" s="2" t="inlineStr">
         <is>
-          <t>VMAAYMAR</t>
+          <t>VMAENINF</t>
         </is>
       </c>
       <c r="H74" s="2" t="inlineStr">
         <is>
-          <t>SORIA, ANA PAULA</t>
+          <t>GOMEZ, AYLEN MILAGROS</t>
         </is>
       </c>
     </row>
@@ -3178,18 +3030,18 @@
       </c>
       <c r="B75" s="5" t="inlineStr">
         <is>
-          <t>MARTINEZ IGNACIO</t>
+          <t>MACHADO RIVERA ELIAS RAUL</t>
         </is>
       </c>
       <c r="C75" s="5" t="n">
-        <v>605696</v>
+        <v>606463</v>
       </c>
       <c r="D75" s="2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E75" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>19:30 - 20:00</t>
         </is>
       </c>
       <c r="F75" s="2" t="n">
@@ -3197,12 +3049,12 @@
       </c>
       <c r="G75" s="2" t="inlineStr">
         <is>
-          <t>VMAIGMAR</t>
+          <t>VMAELMAC</t>
         </is>
       </c>
       <c r="H75" s="2" t="inlineStr">
         <is>
-          <t>VILLALBA, VICTORIA</t>
+          <t>GOYECHEA, AGUSTINA LOURDES</t>
         </is>
       </c>
     </row>
@@ -3214,18 +3066,18 @@
       </c>
       <c r="B76" s="5" t="inlineStr">
         <is>
-          <t>MENGUEZ LUKA PATRICIO</t>
+          <t>MAIDANA MENDOZA MALENA MELISA</t>
         </is>
       </c>
       <c r="C76" s="5" t="n">
-        <v>606123</v>
+        <v>605513</v>
       </c>
       <c r="D76" s="2" t="n">
         <v>13</v>
       </c>
       <c r="E76" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 17:30</t>
+          <t>14:00 - 18:00</t>
         </is>
       </c>
       <c r="F76" s="2" t="n">
@@ -3233,12 +3085,12 @@
       </c>
       <c r="G76" s="2" t="inlineStr">
         <is>
-          <t>VMALUMEN</t>
+          <t>VMAMAMAI</t>
         </is>
       </c>
       <c r="H76" s="2" t="inlineStr">
         <is>
-          <t>LOUREIRO, FLORENCIA CANDELA</t>
+          <t>YBARRA, LUCIA ALDANA</t>
         </is>
       </c>
     </row>
@@ -3250,18 +3102,18 @@
       </c>
       <c r="B77" s="5" t="inlineStr">
         <is>
-          <t>MIRAGAYA MARIA JOSE</t>
+          <t>MAIZ CAMILA</t>
         </is>
       </c>
       <c r="C77" s="5" t="n">
-        <v>606437</v>
+        <v>606219</v>
       </c>
       <c r="D77" s="2" t="n">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="E77" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 20:00</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F77" s="2" t="n">
@@ -3269,12 +3121,12 @@
       </c>
       <c r="G77" s="2" t="inlineStr">
         <is>
-          <t>VMAMAMIR</t>
+          <t>VMACAMAI</t>
         </is>
       </c>
       <c r="H77" s="2" t="inlineStr">
         <is>
-          <t>ROJAS, LUCAS</t>
+          <t>ONETTO, MARIA DE LOS MILAGROS</t>
         </is>
       </c>
     </row>
@@ -3286,18 +3138,18 @@
       </c>
       <c r="B78" s="5" t="inlineStr">
         <is>
-          <t>OJEDA MAYRA ALEJANDRA</t>
+          <t>MANFREDI RUTH MELINA</t>
         </is>
       </c>
       <c r="C78" s="5" t="n">
-        <v>606288</v>
+        <v>605632</v>
       </c>
       <c r="D78" s="2" t="n">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="E78" s="2" t="inlineStr">
         <is>
-          <t>18:00 - 20:00</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F78" s="2" t="n">
@@ -3305,7 +3157,7 @@
       </c>
       <c r="G78" s="2" t="inlineStr">
         <is>
-          <t>VMAMAYOJ</t>
+          <t>VMAMEMAN</t>
         </is>
       </c>
       <c r="H78" s="2" t="inlineStr">
@@ -3322,14 +3174,14 @@
       </c>
       <c r="B79" s="5" t="inlineStr">
         <is>
-          <t>NAVARRO BRUNO OCTAVIO</t>
+          <t>MARAZ AYELEN JACQUELINE</t>
         </is>
       </c>
       <c r="C79" s="5" t="n">
-        <v>606049</v>
+        <v>606142</v>
       </c>
       <c r="D79" s="2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E79" s="2" t="inlineStr">
         <is>
@@ -3341,7 +3193,7 @@
       </c>
       <c r="G79" s="2" t="inlineStr">
         <is>
-          <t>VMABRNAV</t>
+          <t>VMAAYMAR</t>
         </is>
       </c>
       <c r="H79" s="2" t="inlineStr">
@@ -3358,18 +3210,18 @@
       </c>
       <c r="B80" s="5" t="inlineStr">
         <is>
-          <t>OLIVARES MIRIAM DANIELA</t>
+          <t>MARTINEZ IGNACIO</t>
         </is>
       </c>
       <c r="C80" s="5" t="n">
-        <v>606026</v>
+        <v>605696</v>
       </c>
       <c r="D80" s="2" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E80" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 15:30</t>
         </is>
       </c>
       <c r="F80" s="2" t="n">
@@ -3377,12 +3229,12 @@
       </c>
       <c r="G80" s="2" t="inlineStr">
         <is>
-          <t>VMAMIOLI</t>
+          <t>VMAIGMAR</t>
         </is>
       </c>
       <c r="H80" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>VILLALBA, VICTORIA</t>
         </is>
       </c>
     </row>
@@ -3394,18 +3246,18 @@
       </c>
       <c r="B81" s="5" t="inlineStr">
         <is>
-          <t>PAEZ LUCAS ENZO GREGORIO</t>
+          <t>MENGUEZ LUKA PATRICIO</t>
         </is>
       </c>
       <c r="C81" s="5" t="n">
-        <v>606285</v>
+        <v>606123</v>
       </c>
       <c r="D81" s="2" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E81" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 17:30</t>
         </is>
       </c>
       <c r="F81" s="2" t="n">
@@ -3413,12 +3265,12 @@
       </c>
       <c r="G81" s="2" t="inlineStr">
         <is>
-          <t>VMALUPAE</t>
+          <t>VMALUMEN</t>
         </is>
       </c>
       <c r="H81" s="2" t="inlineStr">
         <is>
-          <t>ONETTO, MARIA DE LOS MILAGROS</t>
+          <t>LOUREIRO, FLORENCIA CANDELA</t>
         </is>
       </c>
     </row>
@@ -3430,18 +3282,18 @@
       </c>
       <c r="B82" s="5" t="inlineStr">
         <is>
-          <t>PEREZ LOURDES</t>
+          <t>MIRAGAYA MARIA JOSE</t>
         </is>
       </c>
       <c r="C82" s="5" t="n">
-        <v>606058</v>
+        <v>606437</v>
       </c>
       <c r="D82" s="2" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="E82" s="2" t="inlineStr">
         <is>
-          <t>15:30 - 20:00</t>
+          <t>14:00 - 20:00</t>
         </is>
       </c>
       <c r="F82" s="2" t="n">
@@ -3449,12 +3301,12 @@
       </c>
       <c r="G82" s="2" t="inlineStr">
         <is>
-          <t>VMALOPER</t>
+          <t>VMAMAMIR</t>
         </is>
       </c>
       <c r="H82" s="2" t="inlineStr">
         <is>
-          <t>MIR, TOMAS MAURICIO</t>
+          <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
@@ -3466,18 +3318,18 @@
       </c>
       <c r="B83" s="5" t="inlineStr">
         <is>
-          <t>PINO ELISA</t>
+          <t>OJEDA MAYRA ALEJANDRA</t>
         </is>
       </c>
       <c r="C83" s="5" t="n">
-        <v>606370</v>
+        <v>606288</v>
       </c>
       <c r="D83" s="2" t="n">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="E83" s="2" t="inlineStr">
         <is>
-          <t>14:30 - 20:00</t>
+          <t>18:00 - 20:00</t>
         </is>
       </c>
       <c r="F83" s="2" t="n">
@@ -3485,12 +3337,12 @@
       </c>
       <c r="G83" s="2" t="inlineStr">
         <is>
-          <t>VMAELPIN</t>
+          <t>VMAMAYOJ</t>
         </is>
       </c>
       <c r="H83" s="2" t="inlineStr">
         <is>
-          <t>SORIA, ANA PAULA</t>
+          <t>GOMEZ, SASHA</t>
         </is>
       </c>
     </row>
@@ -3502,18 +3354,18 @@
       </c>
       <c r="B84" s="5" t="inlineStr">
         <is>
-          <t>SAGRADO NICOLAS</t>
+          <t>NAVARRO BRUNO OCTAVIO</t>
         </is>
       </c>
       <c r="C84" s="5" t="n">
-        <v>606616</v>
+        <v>606049</v>
       </c>
       <c r="D84" s="2" t="n">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="E84" s="2" t="inlineStr">
         <is>
-          <t>15:00 - 20:00</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F84" s="2" t="n">
@@ -3521,12 +3373,12 @@
       </c>
       <c r="G84" s="2" t="inlineStr">
         <is>
-          <t>VMANISAG</t>
+          <t>VMABRNAV</t>
         </is>
       </c>
       <c r="H84" s="2" t="inlineStr">
         <is>
-          <t>SOLER, SANTIAGO MAXIMILIANO</t>
+          <t>SORIA, ANA PAULA</t>
         </is>
       </c>
     </row>
@@ -3538,18 +3390,18 @@
       </c>
       <c r="B85" s="5" t="inlineStr">
         <is>
-          <t>SALLES MATIAS</t>
+          <t>OLIVARES MIRIAM DANIELA</t>
         </is>
       </c>
       <c r="C85" s="5" t="n">
-        <v>606644</v>
+        <v>606026</v>
       </c>
       <c r="D85" s="2" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="E85" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 14:30</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F85" s="2" t="n">
@@ -3557,12 +3409,12 @@
       </c>
       <c r="G85" s="2" t="inlineStr">
         <is>
-          <t>VMAMATSA</t>
+          <t>VMAMIOLI</t>
         </is>
       </c>
       <c r="H85" s="2" t="inlineStr">
         <is>
-          <t>MIR, TOMAS MAURICIO</t>
+          <t>GOMEZ, SASHA</t>
         </is>
       </c>
     </row>
@@ -3574,18 +3426,18 @@
       </c>
       <c r="B86" s="5" t="inlineStr">
         <is>
-          <t>SANCHEZ ADRIAN ALEJANDRO</t>
+          <t>PAEZ LUCAS ENZO GREGORIO</t>
         </is>
       </c>
       <c r="C86" s="5" t="n">
-        <v>606498</v>
+        <v>606285</v>
       </c>
       <c r="D86" s="2" t="n">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E86" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F86" s="2" t="n">
@@ -3593,12 +3445,12 @@
       </c>
       <c r="G86" s="2" t="inlineStr">
         <is>
-          <t>VMAADSAN</t>
+          <t>VMALUPAE</t>
         </is>
       </c>
       <c r="H86" s="2" t="inlineStr">
         <is>
-          <t>LOUREIRO, FLORENCIA CANDELA</t>
+          <t>ONETTO, MARIA DE LOS MILAGROS</t>
         </is>
       </c>
     </row>
@@ -3610,18 +3462,18 @@
       </c>
       <c r="B87" s="5" t="inlineStr">
         <is>
-          <t>SANCHEZ JUAN MARCELO</t>
+          <t>PEREZ LOURDES</t>
         </is>
       </c>
       <c r="C87" s="5" t="n">
-        <v>606646</v>
+        <v>606058</v>
       </c>
       <c r="D87" s="2" t="n">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E87" s="2" t="inlineStr">
         <is>
-          <t>18:00 - 20:00</t>
+          <t>15:30 - 20:00</t>
         </is>
       </c>
       <c r="F87" s="2" t="n">
@@ -3629,7 +3481,7 @@
       </c>
       <c r="G87" s="2" t="inlineStr">
         <is>
-          <t>VMAJUSAN</t>
+          <t>VMALOPER</t>
         </is>
       </c>
       <c r="H87" s="2" t="inlineStr">
@@ -3646,18 +3498,18 @@
       </c>
       <c r="B88" s="5" t="inlineStr">
         <is>
-          <t>SOSA LUCIA CELESTE</t>
+          <t>PINO ELISA</t>
         </is>
       </c>
       <c r="C88" s="5" t="n">
-        <v>605912</v>
+        <v>606370</v>
       </c>
       <c r="D88" s="2" t="n">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E88" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>14:30 - 20:00</t>
         </is>
       </c>
       <c r="F88" s="2" t="n">
@@ -3665,12 +3517,12 @@
       </c>
       <c r="G88" s="2" t="inlineStr">
         <is>
-          <t>VMASOLUC</t>
+          <t>VMAELPIN</t>
         </is>
       </c>
       <c r="H88" s="2" t="inlineStr">
         <is>
-          <t>LOUREIRO, FLORENCIA CANDELA</t>
+          <t>SORIA, ANA PAULA</t>
         </is>
       </c>
     </row>
@@ -3682,18 +3534,18 @@
       </c>
       <c r="B89" s="5" t="inlineStr">
         <is>
-          <t>SOSA VALENTINA</t>
+          <t>SAGRADO NICOLAS</t>
         </is>
       </c>
       <c r="C89" s="5" t="n">
-        <v>605769</v>
+        <v>606616</v>
       </c>
       <c r="D89" s="2" t="n">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="E89" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:00</t>
+          <t>15:00 - 20:00</t>
         </is>
       </c>
       <c r="F89" s="2" t="n">
@@ -3701,12 +3553,12 @@
       </c>
       <c r="G89" s="2" t="inlineStr">
         <is>
-          <t>VMAVASOS</t>
+          <t>VMANISAG</t>
         </is>
       </c>
       <c r="H89" s="2" t="inlineStr">
         <is>
-          <t>ROBLEDO, LEANDRO JAVIER</t>
+          <t>SOLER, SANTIAGO MAXIMILIANO</t>
         </is>
       </c>
     </row>
@@ -3718,18 +3570,18 @@
       </c>
       <c r="B90" s="5" t="inlineStr">
         <is>
-          <t>SOTOS LA IACONA ENZO SANTINO</t>
+          <t>SALLES MATIAS</t>
         </is>
       </c>
       <c r="C90" s="5" t="n">
-        <v>605612</v>
+        <v>606644</v>
       </c>
       <c r="D90" s="2" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E90" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:00 - 14:30</t>
         </is>
       </c>
       <c r="F90" s="2" t="n">
@@ -3737,12 +3589,12 @@
       </c>
       <c r="G90" s="2" t="inlineStr">
         <is>
-          <t>VMAENSOT</t>
+          <t>VMAMATSA</t>
         </is>
       </c>
       <c r="H90" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>MIR, TOMAS MAURICIO</t>
         </is>
       </c>
     </row>
@@ -3754,18 +3606,18 @@
       </c>
       <c r="B91" s="5" t="inlineStr">
         <is>
-          <t>VALENZUELA MELINA GISELLE</t>
+          <t>SANCHEZ ADRIAN ALEJANDRO</t>
         </is>
       </c>
       <c r="C91" s="5" t="n">
-        <v>605545</v>
+        <v>606498</v>
       </c>
       <c r="D91" s="2" t="n">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="E91" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:30</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F91" s="2" t="n">
@@ -3773,12 +3625,12 @@
       </c>
       <c r="G91" s="2" t="inlineStr">
         <is>
-          <t>VMAMEVAL</t>
+          <t>VMAADSAN</t>
         </is>
       </c>
       <c r="H91" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>LOUREIRO, FLORENCIA CANDELA</t>
         </is>
       </c>
     </row>
@@ -3790,18 +3642,18 @@
       </c>
       <c r="B92" s="5" t="inlineStr">
         <is>
-          <t>VARGAS CAROLINA MELANY</t>
+          <t>SANCHEZ JUAN MARCELO</t>
         </is>
       </c>
       <c r="C92" s="5" t="n">
-        <v>605957</v>
+        <v>606646</v>
       </c>
       <c r="D92" s="2" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E92" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>18:00 - 20:00</t>
         </is>
       </c>
       <c r="F92" s="2" t="n">
@@ -3809,12 +3661,12 @@
       </c>
       <c r="G92" s="2" t="inlineStr">
         <is>
-          <t>VMACAVAR</t>
+          <t>VMAJUSAN</t>
         </is>
       </c>
       <c r="H92" s="2" t="inlineStr">
         <is>
-          <t>GROESMANN, MAYA JUDITH</t>
+          <t>MIR, TOMAS MAURICIO</t>
         </is>
       </c>
     </row>
@@ -3826,18 +3678,18 @@
       </c>
       <c r="B93" s="5" t="inlineStr">
         <is>
-          <t>VAZQUEZ ROSSI SOFIA ANAHI</t>
+          <t>SOSA LUCIA CELESTE</t>
         </is>
       </c>
       <c r="C93" s="5" t="n">
-        <v>605794</v>
+        <v>605912</v>
       </c>
       <c r="D93" s="2" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="E93" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 15:30</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F93" s="2" t="n">
@@ -3845,12 +3697,12 @@
       </c>
       <c r="G93" s="2" t="inlineStr">
         <is>
-          <t>VMASOVAZ</t>
+          <t>VMASOLUC</t>
         </is>
       </c>
       <c r="H93" s="2" t="inlineStr">
         <is>
-          <t>GOMEZ, SASHA</t>
+          <t>LOUREIRO, FLORENCIA CANDELA</t>
         </is>
       </c>
     </row>
@@ -3862,18 +3714,18 @@
       </c>
       <c r="B94" s="5" t="inlineStr">
         <is>
-          <t>ZALAZAR BRAIAN EDGARDO</t>
+          <t>SOSA VALENTINA</t>
         </is>
       </c>
       <c r="C94" s="5" t="n">
-        <v>609727</v>
+        <v>605769</v>
       </c>
       <c r="D94" s="2" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
-          <t>14:00 - 16:30</t>
+          <t>14:00 - 15:00</t>
         </is>
       </c>
       <c r="F94" s="2" t="n">
@@ -3881,7 +3733,7 @@
       </c>
       <c r="G94" s="2" t="inlineStr">
         <is>
-          <t>VMABRZAL</t>
+          <t>VMAVASOS</t>
         </is>
       </c>
       <c r="H94" s="2" t="inlineStr">
@@ -3898,35 +3750,218 @@
       </c>
       <c r="B95" s="5" t="inlineStr">
         <is>
+          <t>SOTOS LA IACONA ENZO SANTINO</t>
+        </is>
+      </c>
+      <c r="C95" s="5" t="n">
+        <v>605612</v>
+      </c>
+      <c r="D95" s="2" t="n">
+        <v>22</v>
+      </c>
+      <c r="E95" s="2" t="inlineStr">
+        <is>
+          <t>14:00 - 15:30</t>
+        </is>
+      </c>
+      <c r="F95" s="2" t="n">
+        <v/>
+      </c>
+      <c r="G95" s="2" t="inlineStr">
+        <is>
+          <t>VMAENSOT</t>
+        </is>
+      </c>
+      <c r="H95" s="2" t="inlineStr">
+        <is>
+          <t>GOMEZ, SASHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="inlineStr">
+        <is>
+          <t>S2S PREMIUM</t>
+        </is>
+      </c>
+      <c r="B96" s="5" t="inlineStr">
+        <is>
+          <t>VALENZUELA MELINA GISELLE</t>
+        </is>
+      </c>
+      <c r="C96" s="5" t="n">
+        <v>605545</v>
+      </c>
+      <c r="D96" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="E96" s="2" t="inlineStr">
+        <is>
+          <t>14:00 - 16:30</t>
+        </is>
+      </c>
+      <c r="F96" s="2" t="n">
+        <v/>
+      </c>
+      <c r="G96" s="2" t="inlineStr">
+        <is>
+          <t>VMAMEVAL</t>
+        </is>
+      </c>
+      <c r="H96" s="2" t="inlineStr">
+        <is>
+          <t>GOMEZ, SASHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="inlineStr">
+        <is>
+          <t>S2S PREMIUM</t>
+        </is>
+      </c>
+      <c r="B97" s="5" t="inlineStr">
+        <is>
+          <t>VARGAS CAROLINA MELANY</t>
+        </is>
+      </c>
+      <c r="C97" s="5" t="n">
+        <v>605957</v>
+      </c>
+      <c r="D97" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E97" s="2" t="inlineStr">
+        <is>
+          <t>14:00 - 15:30</t>
+        </is>
+      </c>
+      <c r="F97" s="2" t="n">
+        <v/>
+      </c>
+      <c r="G97" s="2" t="inlineStr">
+        <is>
+          <t>VMACAVAR</t>
+        </is>
+      </c>
+      <c r="H97" s="2" t="inlineStr">
+        <is>
+          <t>GROESMANN, MAYA JUDITH</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="inlineStr">
+        <is>
+          <t>S2S PREMIUM</t>
+        </is>
+      </c>
+      <c r="B98" s="5" t="inlineStr">
+        <is>
+          <t>VAZQUEZ ROSSI SOFIA ANAHI</t>
+        </is>
+      </c>
+      <c r="C98" s="5" t="n">
+        <v>605794</v>
+      </c>
+      <c r="D98" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="E98" s="2" t="inlineStr">
+        <is>
+          <t>14:00 - 15:30</t>
+        </is>
+      </c>
+      <c r="F98" s="2" t="n">
+        <v/>
+      </c>
+      <c r="G98" s="2" t="inlineStr">
+        <is>
+          <t>VMASOVAZ</t>
+        </is>
+      </c>
+      <c r="H98" s="2" t="inlineStr">
+        <is>
+          <t>GOMEZ, SASHA</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="inlineStr">
+        <is>
+          <t>S2S PREMIUM</t>
+        </is>
+      </c>
+      <c r="B99" s="5" t="inlineStr">
+        <is>
+          <t>ZALAZAR BRAIAN EDGARDO</t>
+        </is>
+      </c>
+      <c r="C99" s="5" t="n">
+        <v>609727</v>
+      </c>
+      <c r="D99" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="E99" s="2" t="inlineStr">
+        <is>
+          <t>14:00 - 16:30</t>
+        </is>
+      </c>
+      <c r="F99" s="2" t="n">
+        <v/>
+      </c>
+      <c r="G99" s="2" t="inlineStr">
+        <is>
+          <t>VMABRZAL</t>
+        </is>
+      </c>
+      <c r="H99" s="2" t="inlineStr">
+        <is>
+          <t>ROBLEDO, LEANDRO JAVIER</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="inlineStr">
+        <is>
+          <t>S2S PREMIUM</t>
+        </is>
+      </c>
+      <c r="B100" s="5" t="inlineStr">
+        <is>
           <t>GILLES MORENA</t>
         </is>
       </c>
-      <c r="C95" s="5" t="n">
+      <c r="C100" s="5" t="n">
         <v>605694</v>
       </c>
-      <c r="D95" s="2" t="n">
+      <c r="D100" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="E95" s="2" t="inlineStr">
+      <c r="E100" s="2" t="inlineStr">
         <is>
           <t>00:00 - 00:00</t>
         </is>
       </c>
-      <c r="F95" s="2" t="n">
-        <v/>
-      </c>
-      <c r="G95" s="2" t="inlineStr">
+      <c r="F100" s="2" t="n">
+        <v/>
+      </c>
+      <c r="G100" s="2" t="inlineStr">
         <is>
           <t>VMAMOGIL</t>
         </is>
       </c>
-      <c r="H95" s="2" t="inlineStr">
+      <c r="H100" s="2" t="inlineStr">
         <is>
           <t>ROJAS, LUCAS</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:G4"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>